<commit_message>
Added ability to email participants their secret santa using dummy email address
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Particpants</t>
   </si>
@@ -50,13 +50,7 @@
     <t>Banned givers</t>
   </si>
   <si>
-    <t>alasdair.winter@fail.com</t>
-  </si>
-  <si>
-    <t>alasdair.winter@fake.com</t>
-  </si>
-  <si>
-    <t>alasdair.winter@fake.comzzzaassssaasvbvdjk</t>
+    <t>example@mail.com</t>
   </si>
 </sst>
 </file>
@@ -112,10 +106,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -400,13 +394,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
     <col min="3" max="3" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -417,28 +411,28 @@
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -448,16 +442,16 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -467,7 +461,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -475,12 +469,7 @@
   <mergeCells count="1">
     <mergeCell ref="C1:G1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>